<commit_message>
added Chinese and Japanese version (part 1)
</commit_message>
<xml_diff>
--- a/_ux/弁護士紹介 中＋日＋英.xlsx
+++ b/_ux/弁護士紹介 中＋日＋英.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9720" activeTab="3"/>
+    <workbookView xWindow="2655" yWindow="75" windowWidth="20745" windowHeight="11130" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Fukuoka" sheetId="1" r:id="rId1"/>
@@ -141,7 +141,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -341,7 +341,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -352,7 +352,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -362,7 +362,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -483,7 +483,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -509,7 +509,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -521,7 +521,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -532,7 +532,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -543,7 +543,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -554,7 +554,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -565,7 +565,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -575,7 +575,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -587,7 +587,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -598,7 +598,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -609,7 +609,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -619,7 +619,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -630,7 +630,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -710,7 +710,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -745,7 +745,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -756,7 +756,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -767,7 +767,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -858,7 +858,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -960,7 +960,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1078,7 +1078,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1089,7 +1089,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1100,7 +1100,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1111,7 +1111,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1122,7 +1122,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1295,7 +1295,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1306,7 +1306,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1401,10 +1401,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Kyo　Masataka</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>紹介文</t>
     <rPh sb="0" eb="2">
       <t>ショウカイ</t>
@@ -1444,7 +1440,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1513,7 +1509,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1596,7 +1592,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1607,7 +1603,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1730,7 +1726,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1757,7 +1753,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1789,7 +1785,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1857,7 +1853,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -1869,7 +1865,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1880,7 +1876,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -1891,7 +1887,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1903,7 +1899,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -1914,7 +1910,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1926,7 +1922,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -1937,7 +1933,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1954,7 +1950,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1965,7 +1961,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1975,7 +1971,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1986,7 +1982,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1996,7 +1992,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2007,7 +2003,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2017,7 +2013,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2028,7 +2024,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2038,7 +2034,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2049,7 +2045,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2060,7 +2056,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2071,7 +2067,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2082,7 +2078,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2093,7 +2089,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2103,7 +2099,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2114,7 +2110,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2124,7 +2120,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2137,7 +2133,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2147,7 +2143,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2158,7 +2154,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2168,7 +2164,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2179,7 +2175,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2189,7 +2185,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2200,7 +2196,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2210,7 +2206,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2227,7 +2223,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2238,7 +2234,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2248,7 +2244,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2259,7 +2255,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2270,7 +2266,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2281,7 +2277,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2291,7 +2287,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2302,7 +2298,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2313,7 +2309,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2324,7 +2320,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2361,7 +2357,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2371,7 +2367,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2382,7 +2378,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2400,7 +2396,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2411,7 +2407,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2421,7 +2417,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2432,7 +2428,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2443,7 +2439,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2454,7 +2450,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2464,7 +2460,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2475,7 +2471,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2486,7 +2482,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2497,7 +2493,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2507,7 +2503,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2518,7 +2514,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2540,7 +2536,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2551,7 +2547,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2562,7 +2558,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2573,7 +2569,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2584,7 +2580,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2595,7 +2591,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2606,7 +2602,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2617,7 +2613,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2628,7 +2624,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2639,7 +2635,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2650,7 +2646,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2661,7 +2657,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2672,7 +2668,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2683,7 +2679,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2694,7 +2690,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2705,7 +2701,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2716,7 +2712,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2726,7 +2722,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2737,7 +2733,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2747,7 +2743,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2758,7 +2754,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2768,7 +2764,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2779,7 +2775,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2789,7 +2785,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2800,7 +2796,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2811,7 +2807,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2822,7 +2818,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2833,7 +2829,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2844,7 +2840,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2854,7 +2850,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2865,7 +2861,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2876,7 +2872,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2887,7 +2883,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2898,7 +2894,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2909,7 +2905,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2920,7 +2916,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2931,7 +2927,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2942,7 +2938,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2953,7 +2949,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2964,7 +2960,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2975,7 +2971,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2986,7 +2982,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2996,7 +2992,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3007,7 +3003,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -3017,7 +3013,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3028,16 +3024,12 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>）</t>
     </r>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>"Explicate the Nationality Law of South Korean one by one" (Akashi Publication 2014)</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -3106,7 +3098,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3191,7 +3183,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3210,7 +3202,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3221,7 +3213,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3233,7 +3225,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3244,7 +3236,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3255,7 +3247,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3266,7 +3258,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3278,7 +3270,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3289,7 +3281,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3300,7 +3292,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3311,7 +3303,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3323,7 +3315,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3334,7 +3326,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3345,7 +3337,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3356,7 +3348,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3367,7 +3359,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3378,7 +3370,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -3389,7 +3381,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3400,7 +3392,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3411,7 +3403,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3422,7 +3414,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3433,7 +3425,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3444,7 +3436,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3455,7 +3447,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3466,7 +3458,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3477,7 +3469,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3488,7 +3480,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3500,7 +3492,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3511,7 +3503,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3522,7 +3514,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3533,7 +3525,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3544,7 +3536,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3555,7 +3547,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3567,7 +3559,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3578,7 +3570,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3589,7 +3581,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3600,7 +3592,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3611,7 +3603,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3622,7 +3614,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3640,7 +3632,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3651,7 +3643,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -3663,7 +3655,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3674,7 +3666,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -3684,7 +3676,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3695,7 +3687,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -3721,7 +3713,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3737,7 +3729,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3756,7 +3748,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3767,7 +3759,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3778,7 +3770,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3789,7 +3781,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3801,7 +3793,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3812,7 +3804,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3823,7 +3815,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3834,7 +3826,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3845,7 +3837,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3856,7 +3848,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3867,7 +3859,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3878,7 +3870,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3889,7 +3881,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3900,7 +3892,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3911,7 +3903,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3922,7 +3914,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3934,7 +3926,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3945,7 +3937,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3956,7 +3948,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3967,7 +3959,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3978,7 +3970,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3989,7 +3981,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -4001,7 +3993,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -4018,7 +4010,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -4045,7 +4037,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -4056,24 +4048,55 @@
   </si>
   <si>
     <t>Total Chie Representive</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>Kyo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>u</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>　Masataka</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Commentary on Korean Nationality Law-Yasuhiro Okuda, Katsuhiko Oka, Masataka Kyou -Akashi Publication 2014</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -4081,7 +4104,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -4095,7 +4118,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -4103,7 +4126,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -4111,7 +4134,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -4133,7 +4156,7 @@
       <b/>
       <sz val="18"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -4141,7 +4164,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -4150,7 +4173,7 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -4158,14 +4181,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -4173,20 +4196,20 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4235,6 +4258,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="38">
     <border>
@@ -4739,7 +4768,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="165">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4774,24 +4803,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -4819,24 +4830,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -4867,24 +4860,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -4915,21 +4890,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -4963,9 +4923,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -4990,66 +4947,33 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5059,67 +4983,10 @@
     <xf numFmtId="0" fontId="15" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -5151,24 +5018,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5223,9 +5072,99 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -5241,7 +5180,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office ​​テーマ">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -5283,7 +5222,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5316,26 +5255,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5368,23 +5290,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -5561,44 +5466,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView showGridLines="0" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="11.46484375" customWidth="1"/>
-    <col min="2" max="2" width="19.46484375" customWidth="1"/>
-    <col min="3" max="3" width="19.86328125" customWidth="1"/>
-    <col min="4" max="4" width="21.1328125" customWidth="1"/>
-    <col min="5" max="5" width="26.1328125" customWidth="1"/>
-    <col min="6" max="6" width="50.46484375" customWidth="1"/>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="2" max="2" width="19.5" customWidth="1"/>
+    <col min="3" max="3" width="19.875" customWidth="1"/>
+    <col min="4" max="4" width="21.125" customWidth="1"/>
+    <col min="5" max="5" width="26.125" customWidth="1"/>
+    <col min="6" max="6" width="50.5" customWidth="1"/>
     <col min="7" max="7" width="69" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="A1" s="79"/>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
+      <c r="A1" s="55"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="80" t="s">
+      <c r="D1" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="80" t="s">
+      <c r="E1" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="80" t="s">
+      <c r="F1" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="81" t="s">
+      <c r="G1" s="57" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="93" customHeight="1">
-      <c r="A2" s="147" t="s">
+    <row r="2" spans="1:7" ht="93" customHeight="1">
+      <c r="A2" s="87" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -5614,19 +5519,16 @@
         <v>17</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G2" s="82" t="s">
-        <v>133</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
+        <v>128</v>
+      </c>
+      <c r="G2" s="58" t="s">
+        <v>132</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="111" customHeight="1">
-      <c r="A3" s="148"/>
+    <row r="3" spans="1:7" ht="111" customHeight="1">
+      <c r="A3" s="88"/>
       <c r="B3" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>6</v>
@@ -5638,287 +5540,275 @@
         <v>15</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="G3" s="83" t="s">
+        <v>131</v>
+      </c>
+      <c r="G3" s="59" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="96.75" customHeight="1" thickBot="1">
+      <c r="A4" s="88"/>
+      <c r="B4" s="105" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="106" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="107" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="108" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="109" t="s">
+        <v>164</v>
+      </c>
+      <c r="G4" s="110" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="67.5">
+      <c r="A5" s="88"/>
+      <c r="B5" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="60" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="94.5">
+      <c r="A6" s="88"/>
+      <c r="B6" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="G6" s="61" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="68.25" thickBot="1">
+      <c r="A7" s="88"/>
+      <c r="B7" s="105" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="106" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" s="107" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="108" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="111" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="112" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="67.5">
+      <c r="A8" s="88"/>
+      <c r="B8" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="23"/>
+      <c r="E8" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="G8" s="62" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="63.75" customHeight="1">
+      <c r="A9" s="88"/>
+      <c r="B9" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="G9" s="63" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="66.75" customHeight="1" thickBot="1">
+      <c r="A10" s="88"/>
+      <c r="B10" s="105" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="106" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="107"/>
+      <c r="E10" s="108" t="s">
+        <v>163</v>
+      </c>
+      <c r="F10" s="111" t="s">
+        <v>178</v>
+      </c>
+      <c r="G10" s="113" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="81">
+      <c r="A11" s="88"/>
+      <c r="B11" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="G11" s="64" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="67.5" customHeight="1">
+      <c r="A12" s="88"/>
+      <c r="B12" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>189</v>
+      </c>
+      <c r="D12" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="36" t="s">
+        <v>96</v>
+      </c>
+      <c r="G12" s="65" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="74.25" customHeight="1" thickBot="1">
+      <c r="A13" s="88"/>
+      <c r="B13" s="105" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="106" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="107" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="108" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="111" t="s">
+        <v>124</v>
+      </c>
+      <c r="G13" s="114" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="243">
+      <c r="A14" s="89" t="s">
+        <v>134</v>
+      </c>
+      <c r="B14" s="77" t="s">
+        <v>135</v>
+      </c>
+      <c r="C14" s="78" t="s">
+        <v>136</v>
+      </c>
+      <c r="D14" s="79"/>
+      <c r="E14" s="78" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="80" t="s">
+        <v>137</v>
+      </c>
+      <c r="G14" s="81" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="267.75" customHeight="1">
+      <c r="A15" s="90"/>
+      <c r="B15" s="82" t="s">
         <v>171</v>
       </c>
+      <c r="C15" s="83" t="s">
+        <v>139</v>
+      </c>
+      <c r="D15" s="84"/>
+      <c r="E15" s="83" t="s">
+        <v>165</v>
+      </c>
+      <c r="F15" s="85" t="s">
+        <v>168</v>
+      </c>
+      <c r="G15" s="86" t="s">
+        <v>170</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" ht="96.75" customHeight="1" thickBot="1">
-      <c r="A4" s="148"/>
-      <c r="B4" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>165</v>
-      </c>
-      <c r="G4" s="84" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="71.25">
-      <c r="A5" s="148"/>
-      <c r="B5" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="85" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="99.75">
-      <c r="A6" s="148"/>
-      <c r="B6" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="25" t="s">
-        <v>122</v>
-      </c>
-      <c r="G6" s="86" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="71.650000000000006" thickBot="1">
-      <c r="A7" s="148"/>
-      <c r="B7" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="D7" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" s="87" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="85.5">
-      <c r="A8" s="148"/>
-      <c r="B8" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="98" t="s">
-        <v>178</v>
-      </c>
-      <c r="G8" s="88" t="s">
-        <v>130</v>
-      </c>
-      <c r="H8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="63.75" customHeight="1">
-      <c r="A9" s="148"/>
-      <c r="B9" s="38" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="39" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9" s="41" t="s">
+    <row r="16" spans="1:7" ht="204.75" customHeight="1">
+      <c r="A16" s="91"/>
+      <c r="B16" s="115" t="s">
+        <v>138</v>
+      </c>
+      <c r="C16" s="116" t="s">
+        <v>140</v>
+      </c>
+      <c r="D16" s="117"/>
+      <c r="E16" s="118" t="s">
+        <v>102</v>
+      </c>
+      <c r="F16" s="119" t="s">
         <v>179</v>
       </c>
-      <c r="G9" s="89" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="66.75" customHeight="1" thickBot="1">
-      <c r="A10" s="148"/>
-      <c r="B10" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="45"/>
-      <c r="E10" s="46" t="s">
-        <v>164</v>
-      </c>
-      <c r="F10" s="47" t="s">
-        <v>180</v>
-      </c>
-      <c r="G10" s="90" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="85.5">
-      <c r="A11" s="148"/>
-      <c r="B11" s="55" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="49" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="50" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="49" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="51" t="s">
-        <v>95</v>
-      </c>
-      <c r="G11" s="91" t="s">
-        <v>131</v>
-      </c>
-      <c r="H11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="67.5" customHeight="1">
-      <c r="A12" s="148"/>
-      <c r="B12" s="57" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="52" t="s">
-        <v>110</v>
-      </c>
-      <c r="D12" s="53" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="52" t="s">
-        <v>40</v>
-      </c>
-      <c r="F12" s="54" t="s">
-        <v>96</v>
-      </c>
-      <c r="G12" s="92" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="74.25" customHeight="1" thickBot="1">
-      <c r="A13" s="148"/>
-      <c r="B13" s="59" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="60" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="61" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="62" t="s">
-        <v>41</v>
-      </c>
-      <c r="F13" s="63" t="s">
-        <v>125</v>
-      </c>
-      <c r="G13" s="93" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="299.25">
-      <c r="A14" s="149" t="s">
-        <v>135</v>
-      </c>
-      <c r="B14" s="131" t="s">
-        <v>136</v>
-      </c>
-      <c r="C14" s="132" t="s">
-        <v>137</v>
-      </c>
-      <c r="D14" s="133"/>
-      <c r="E14" s="132" t="s">
-        <v>17</v>
-      </c>
-      <c r="F14" s="134" t="s">
-        <v>138</v>
-      </c>
-      <c r="G14" s="135" t="s">
-        <v>175</v>
-      </c>
-      <c r="H14">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="267.75" customHeight="1">
-      <c r="A15" s="150"/>
-      <c r="B15" s="136" t="s">
-        <v>173</v>
-      </c>
-      <c r="C15" s="137" t="s">
-        <v>140</v>
-      </c>
-      <c r="D15" s="138"/>
-      <c r="E15" s="137" t="s">
-        <v>166</v>
-      </c>
-      <c r="F15" s="139" t="s">
-        <v>170</v>
-      </c>
-      <c r="G15" s="140" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="204.75" customHeight="1">
-      <c r="A16" s="151"/>
-      <c r="B16" s="141" t="s">
-        <v>139</v>
-      </c>
-      <c r="C16" s="142" t="s">
-        <v>141</v>
-      </c>
-      <c r="D16" s="143"/>
-      <c r="E16" s="144" t="s">
-        <v>102</v>
-      </c>
-      <c r="F16" s="145" t="s">
-        <v>181</v>
-      </c>
-      <c r="G16" s="146" t="s">
-        <v>176</v>
+      <c r="G16" s="120" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -5934,44 +5824,44 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="B16" sqref="B16:G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="11.46484375" customWidth="1"/>
-    <col min="2" max="2" width="19.46484375" customWidth="1"/>
-    <col min="3" max="3" width="19.86328125" customWidth="1"/>
-    <col min="4" max="4" width="23.86328125" customWidth="1"/>
-    <col min="5" max="5" width="26.1328125" customWidth="1"/>
-    <col min="6" max="6" width="52.86328125" customWidth="1"/>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="2" max="2" width="19.5" customWidth="1"/>
+    <col min="3" max="3" width="19.875" customWidth="1"/>
+    <col min="4" max="4" width="23.875" customWidth="1"/>
+    <col min="5" max="5" width="26.125" customWidth="1"/>
+    <col min="6" max="6" width="52.875" customWidth="1"/>
     <col min="7" max="7" width="69" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="34.5" customHeight="1" thickBot="1">
-      <c r="A1" s="104"/>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105" t="s">
+    <row r="1" spans="1:7" ht="34.5" customHeight="1" thickBot="1">
+      <c r="A1" s="69"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="106" t="s">
+      <c r="D1" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="106" t="s">
+      <c r="E1" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="106" t="s">
+      <c r="F1" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="106" t="s">
+      <c r="G1" s="71" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="120" customHeight="1" thickBot="1">
-      <c r="A2" s="147" t="s">
+    <row r="2" spans="1:7" ht="120" customHeight="1" thickBot="1">
+      <c r="A2" s="87" t="s">
         <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -5992,14 +5882,11 @@
       <c r="G2" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="H2">
-        <v>6</v>
-      </c>
     </row>
-    <row r="3" spans="1:8" ht="136.5" customHeight="1" thickBot="1">
-      <c r="A3" s="148"/>
+    <row r="3" spans="1:7" ht="136.5" customHeight="1" thickBot="1">
+      <c r="A3" s="88"/>
       <c r="B3" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>56</v>
@@ -6011,251 +5898,239 @@
         <v>15</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="G3" s="76" t="s">
-        <v>169</v>
+        <v>181</v>
+      </c>
+      <c r="G3" s="52" t="s">
+        <v>167</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="114" customHeight="1" thickBot="1">
-      <c r="A4" s="148"/>
-      <c r="B4" s="12" t="s">
+    <row r="4" spans="1:7" ht="114" customHeight="1" thickBot="1">
+      <c r="A4" s="88"/>
+      <c r="B4" s="105" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="106" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="107" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="108" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="109" t="s">
         <v>55</v>
       </c>
-      <c r="G4" s="103" t="s">
-        <v>167</v>
+      <c r="G4" s="121" t="s">
+        <v>166</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="77.25" customHeight="1">
-      <c r="A5" s="148"/>
-      <c r="B5" s="18" t="s">
+    <row r="5" spans="1:7" ht="77.25" customHeight="1">
+      <c r="A5" s="88"/>
+      <c r="B5" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="21" t="s">
+      <c r="F5" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="G5" s="85"/>
-      <c r="H5">
-        <v>7</v>
-      </c>
+      <c r="G5" s="60"/>
     </row>
-    <row r="6" spans="1:8" ht="95.25" customHeight="1">
-      <c r="A6" s="148"/>
-      <c r="B6" s="22" t="s">
+    <row r="6" spans="1:7" ht="95.25" customHeight="1">
+      <c r="A6" s="88"/>
+      <c r="B6" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="25" t="s">
+      <c r="F6" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="G6" s="61"/>
+    </row>
+    <row r="7" spans="1:7" ht="84" customHeight="1" thickBot="1">
+      <c r="A7" s="88"/>
+      <c r="B7" s="105" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="106" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="107" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="108" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="111" t="s">
+        <v>61</v>
+      </c>
+      <c r="G7" s="112"/>
+    </row>
+    <row r="8" spans="1:7" ht="62.25" customHeight="1">
+      <c r="A8" s="88"/>
+      <c r="B8" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="G8" s="67"/>
+    </row>
+    <row r="9" spans="1:7" ht="75.75" customHeight="1">
+      <c r="A9" s="88"/>
+      <c r="B9" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="G6" s="86"/>
+      <c r="G9" s="63"/>
     </row>
-    <row r="7" spans="1:8" ht="84" customHeight="1" thickBot="1">
-      <c r="A7" s="148"/>
-      <c r="B7" s="27" t="s">
+    <row r="10" spans="1:7" ht="81.75" customHeight="1" thickBot="1">
+      <c r="A10" s="88"/>
+      <c r="B10" s="105" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="E7" s="30" t="s">
+      <c r="C10" s="106" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="107" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" s="108" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="G7" s="87"/>
+      <c r="F10" s="122" t="s">
+        <v>151</v>
+      </c>
+      <c r="G10" s="112"/>
     </row>
-    <row r="8" spans="1:8" ht="62.25" customHeight="1">
-      <c r="A8" s="148"/>
-      <c r="B8" s="33" t="s">
+    <row r="11" spans="1:7" ht="89.25" customHeight="1">
+      <c r="A11" s="88"/>
+      <c r="B11" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="D8" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="E8" s="34" t="s">
+      <c r="C11" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="G8" s="100"/>
-      <c r="H8">
-        <v>8</v>
-      </c>
+      <c r="F11" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="G11" s="68"/>
     </row>
-    <row r="9" spans="1:8" ht="75.75" customHeight="1">
-      <c r="A9" s="148"/>
-      <c r="B9" s="38" t="s">
+    <row r="12" spans="1:7" ht="104.25" customHeight="1">
+      <c r="A12" s="88"/>
+      <c r="B12" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="39" t="s">
-        <v>63</v>
-      </c>
-      <c r="D9" s="40" t="s">
+      <c r="C12" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="41" t="s">
-        <v>124</v>
-      </c>
-      <c r="G9" s="89"/>
+      <c r="E12" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="F12" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="G12" s="65"/>
     </row>
-    <row r="10" spans="1:8" ht="81.75" customHeight="1" thickBot="1">
-      <c r="A10" s="148"/>
-      <c r="B10" s="43" t="s">
+    <row r="13" spans="1:7" ht="81.75" customHeight="1" thickBot="1">
+      <c r="A13" s="88"/>
+      <c r="B13" s="123" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="44" t="s">
-        <v>66</v>
-      </c>
-      <c r="D10" s="45" t="s">
-        <v>65</v>
-      </c>
-      <c r="E10" s="46" t="s">
+      <c r="C13" s="124" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="125" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="126" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="75" t="s">
+      <c r="F13" s="127" t="s">
         <v>152</v>
       </c>
-      <c r="G10" s="101"/>
+      <c r="G13" s="128"/>
     </row>
-    <row r="11" spans="1:8" ht="89.25" customHeight="1">
-      <c r="A11" s="148"/>
-      <c r="B11" s="55" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="49" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11" s="50" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="51" t="s">
-        <v>73</v>
-      </c>
-      <c r="G11" s="102"/>
-      <c r="H11">
-        <v>9</v>
-      </c>
+    <row r="14" spans="1:7" ht="87.75" customHeight="1">
+      <c r="A14" s="72"/>
+      <c r="B14" s="41" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" s="43"/>
+      <c r="E14" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="F14" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="G14" s="45"/>
     </row>
-    <row r="12" spans="1:8" ht="104.25" customHeight="1">
-      <c r="A12" s="148"/>
-      <c r="B12" s="57" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="52" t="s">
-        <v>70</v>
-      </c>
-      <c r="D12" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="52" t="s">
-        <v>72</v>
-      </c>
-      <c r="F12" s="54" t="s">
-        <v>127</v>
-      </c>
-      <c r="G12" s="92"/>
+    <row r="15" spans="1:7" ht="89.25" customHeight="1">
+      <c r="B15" s="46" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" s="48"/>
+      <c r="E15" s="47" t="s">
+        <v>81</v>
+      </c>
+      <c r="F15" s="49" t="s">
+        <v>153</v>
+      </c>
+      <c r="G15" s="50"/>
     </row>
-    <row r="13" spans="1:8" ht="81.75" customHeight="1" thickBot="1">
-      <c r="A13" s="148"/>
-      <c r="B13" s="107" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="108" t="s">
-        <v>71</v>
-      </c>
-      <c r="D13" s="109" t="s">
-        <v>68</v>
-      </c>
-      <c r="E13" s="110" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="111" t="s">
-        <v>153</v>
-      </c>
-      <c r="G13" s="112"/>
-    </row>
-    <row r="14" spans="1:8" ht="87.75" customHeight="1">
-      <c r="A14" s="113"/>
-      <c r="B14" s="64" t="s">
-        <v>74</v>
-      </c>
-      <c r="C14" s="65" t="s">
-        <v>75</v>
-      </c>
-      <c r="D14" s="66"/>
-      <c r="E14" s="65" t="s">
-        <v>80</v>
-      </c>
-      <c r="F14" s="67" t="s">
-        <v>155</v>
-      </c>
-      <c r="G14" s="68"/>
-      <c r="H14">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="89.25" customHeight="1">
-      <c r="B15" s="69" t="s">
-        <v>76</v>
-      </c>
-      <c r="C15" s="70" t="s">
-        <v>79</v>
-      </c>
-      <c r="D15" s="71"/>
-      <c r="E15" s="70" t="s">
-        <v>81</v>
-      </c>
-      <c r="F15" s="72" t="s">
-        <v>154</v>
-      </c>
-      <c r="G15" s="73"/>
-    </row>
-    <row r="16" spans="1:8" ht="108" customHeight="1">
-      <c r="A16" s="114"/>
+    <row r="16" spans="1:7" ht="108" customHeight="1">
+      <c r="A16" s="73"/>
       <c r="B16" s="115" t="s">
         <v>77</v>
       </c>
@@ -6266,10 +6141,10 @@
       <c r="E16" s="118" t="s">
         <v>82</v>
       </c>
-      <c r="F16" s="119" t="s">
-        <v>156</v>
-      </c>
-      <c r="G16" s="120"/>
+      <c r="F16" s="129" t="s">
+        <v>155</v>
+      </c>
+      <c r="G16" s="130"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6282,48 +6157,48 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView showGridLines="0" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="11.46484375" customWidth="1"/>
-    <col min="2" max="2" width="19.46484375" customWidth="1"/>
-    <col min="3" max="3" width="19.86328125" customWidth="1"/>
-    <col min="4" max="4" width="21.1328125" customWidth="1"/>
-    <col min="5" max="5" width="16.59765625" customWidth="1"/>
-    <col min="6" max="6" width="54.59765625" customWidth="1"/>
-    <col min="7" max="7" width="64.3984375" customWidth="1"/>
-    <col min="8" max="8" width="47.265625" customWidth="1"/>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="2" max="2" width="19.5" customWidth="1"/>
+    <col min="3" max="3" width="19.875" customWidth="1"/>
+    <col min="4" max="4" width="21.125" customWidth="1"/>
+    <col min="5" max="5" width="16.625" customWidth="1"/>
+    <col min="6" max="6" width="54.625" customWidth="1"/>
+    <col min="7" max="7" width="64.375" customWidth="1"/>
+    <col min="8" max="8" width="47.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="43.5" customHeight="1" thickBot="1">
-      <c r="A1" s="79"/>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80" t="s">
+    <row r="1" spans="1:8" ht="43.5" customHeight="1" thickBot="1">
+      <c r="A1" s="55"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="80" t="s">
+      <c r="D1" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="80" t="s">
+      <c r="E1" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="80" t="s">
+      <c r="F1" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="80" t="s">
+      <c r="G1" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="81" t="s">
-        <v>111</v>
+      <c r="H1" s="57" t="s">
+        <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="135" customHeight="1">
-      <c r="A2" s="147" t="s">
+    <row r="2" spans="1:8" ht="135" customHeight="1">
+      <c r="A2" s="87" t="s">
         <v>83</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -6341,254 +6216,242 @@
       <c r="F2" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="G2" s="77" t="s">
-        <v>187</v>
-      </c>
-      <c r="H2" s="153" t="s">
+      <c r="G2" s="53" t="s">
+        <v>185</v>
+      </c>
+      <c r="H2" s="93" t="s">
         <v>106</v>
       </c>
-      <c r="I2">
-        <v>11</v>
-      </c>
     </row>
-    <row r="3" spans="1:9" ht="108.75" customHeight="1">
-      <c r="A3" s="148"/>
+    <row r="3" spans="1:8" ht="108.75" customHeight="1">
+      <c r="A3" s="88"/>
       <c r="B3" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>87</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>15</v>
       </c>
       <c r="F3" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="G3" s="54" t="s">
+        <v>172</v>
+      </c>
+      <c r="H3" s="94"/>
+    </row>
+    <row r="4" spans="1:8" ht="147" customHeight="1" thickBot="1">
+      <c r="A4" s="88"/>
+      <c r="B4" s="105" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="106" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" s="107" t="s">
+        <v>94</v>
+      </c>
+      <c r="E4" s="108" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="109" t="s">
+        <v>183</v>
+      </c>
+      <c r="G4" s="131" t="s">
         <v>184</v>
       </c>
-      <c r="G3" s="78" t="s">
-        <v>174</v>
-      </c>
-      <c r="H3" s="154"/>
+      <c r="H4" s="95"/>
     </row>
-    <row r="4" spans="1:9" ht="147" customHeight="1" thickBot="1">
-      <c r="A4" s="148"/>
-      <c r="B4" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="E4" s="15" t="s">
+    <row r="5" spans="1:8" ht="77.25" customHeight="1">
+      <c r="A5" s="88"/>
+      <c r="B5" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="G5" s="51"/>
+      <c r="H5" s="96" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="248.25" customHeight="1">
+      <c r="A6" s="88"/>
+      <c r="B6" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="G6" s="20"/>
+      <c r="H6" s="97"/>
+    </row>
+    <row r="7" spans="1:8" ht="140.25" customHeight="1" thickBot="1">
+      <c r="A7" s="88"/>
+      <c r="B7" s="105" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="106" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" s="107" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" s="108" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="16" t="s">
-        <v>185</v>
-      </c>
-      <c r="G4" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="H4" s="155"/>
+      <c r="F7" s="111" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="131"/>
+      <c r="H7" s="98"/>
     </row>
-    <row r="5" spans="1:9" ht="77.25" customHeight="1">
-      <c r="A5" s="148"/>
-      <c r="B5" s="18" t="s">
+    <row r="8" spans="1:8" ht="140.25" customHeight="1">
+      <c r="A8" s="88"/>
+      <c r="B8" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="E5" s="19" t="s">
+      <c r="C8" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="E8" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="G5" s="74"/>
-      <c r="H5" s="156" t="s">
-        <v>107</v>
-      </c>
-      <c r="I5">
-        <v>12</v>
+      <c r="F8" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="G8" s="25"/>
+      <c r="H8" s="99" t="s">
+        <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="248.25" customHeight="1">
-      <c r="A6" s="148"/>
-      <c r="B6" s="22" t="s">
+    <row r="9" spans="1:8" ht="103.5" customHeight="1">
+      <c r="A9" s="88"/>
+      <c r="B9" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="D6" s="24" t="s">
+      <c r="C9" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="D9" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="E6" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="25" t="s">
+      <c r="E9" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="F9" s="29" t="s">
         <v>146</v>
       </c>
-      <c r="G6" s="26"/>
-      <c r="H6" s="157"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="100"/>
     </row>
-    <row r="7" spans="1:9" ht="140.25" customHeight="1" thickBot="1">
-      <c r="A7" s="148"/>
-      <c r="B7" s="27" t="s">
+    <row r="10" spans="1:8" ht="81.75" customHeight="1" thickBot="1">
+      <c r="A10" s="88"/>
+      <c r="B10" s="105" t="s">
+        <v>150</v>
+      </c>
+      <c r="C10" s="106" t="s">
+        <v>149</v>
+      </c>
+      <c r="D10" s="107" t="s">
+        <v>89</v>
+      </c>
+      <c r="E10" s="108" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="111" t="s">
+        <v>147</v>
+      </c>
+      <c r="G10" s="132"/>
+      <c r="H10" s="101"/>
+    </row>
+    <row r="11" spans="1:8" ht="84.75" customHeight="1">
+      <c r="A11" s="88"/>
+      <c r="B11" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="G11" s="38"/>
+      <c r="H11" s="102" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="94.5" customHeight="1">
+      <c r="A12" s="88"/>
+      <c r="B12" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="D12" s="35" t="s">
+        <v>160</v>
+      </c>
+      <c r="E12" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="F12" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="G12" s="40"/>
+      <c r="H12" s="103"/>
+    </row>
+    <row r="13" spans="1:8" ht="81.75" customHeight="1">
+      <c r="A13" s="92"/>
+      <c r="B13" s="115" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="D7" s="29" t="s">
+      <c r="C13" s="116" t="s">
+        <v>142</v>
+      </c>
+      <c r="D13" s="117" t="s">
         <v>89</v>
       </c>
-      <c r="E7" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" s="32"/>
-      <c r="H7" s="158"/>
-    </row>
-    <row r="8" spans="1:9" ht="140.25" customHeight="1">
-      <c r="A8" s="148"/>
-      <c r="B8" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="D8" s="35" t="s">
-        <v>101</v>
-      </c>
-      <c r="E8" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="36" t="s">
-        <v>100</v>
-      </c>
-      <c r="G8" s="37"/>
-      <c r="H8" s="159" t="s">
-        <v>108</v>
-      </c>
-      <c r="I8">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="103.5" customHeight="1">
-      <c r="A9" s="148"/>
-      <c r="B9" s="38" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="39" t="s">
-        <v>149</v>
-      </c>
-      <c r="D9" s="40" t="s">
-        <v>161</v>
-      </c>
-      <c r="E9" s="39" t="s">
-        <v>103</v>
-      </c>
-      <c r="F9" s="41" t="s">
-        <v>147</v>
-      </c>
-      <c r="G9" s="42"/>
-      <c r="H9" s="160"/>
-    </row>
-    <row r="10" spans="1:9" ht="81.75" customHeight="1" thickBot="1">
-      <c r="A10" s="148"/>
-      <c r="B10" s="43" t="s">
-        <v>151</v>
-      </c>
-      <c r="C10" s="44" t="s">
-        <v>150</v>
-      </c>
-      <c r="D10" s="45" t="s">
-        <v>89</v>
-      </c>
-      <c r="E10" s="46" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="47" t="s">
-        <v>148</v>
-      </c>
-      <c r="G10" s="48"/>
-      <c r="H10" s="161"/>
-    </row>
-    <row r="11" spans="1:9" ht="84.75" customHeight="1">
-      <c r="A11" s="148"/>
-      <c r="B11" s="55" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="49" t="s">
-        <v>104</v>
-      </c>
-      <c r="D11" s="50" t="s">
-        <v>85</v>
-      </c>
-      <c r="E11" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="51" t="s">
-        <v>105</v>
-      </c>
-      <c r="G11" s="56"/>
-      <c r="H11" s="162" t="s">
-        <v>109</v>
-      </c>
-      <c r="I11">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="94.5" customHeight="1">
-      <c r="A12" s="148"/>
-      <c r="B12" s="57" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="52" t="s">
-        <v>142</v>
-      </c>
-      <c r="D12" s="53" t="s">
-        <v>161</v>
-      </c>
-      <c r="E12" s="52" t="s">
-        <v>72</v>
-      </c>
-      <c r="F12" s="54" t="s">
+      <c r="E13" s="118" t="s">
+        <v>102</v>
+      </c>
+      <c r="F13" s="119" t="s">
         <v>144</v>
       </c>
-      <c r="G12" s="58"/>
-      <c r="H12" s="163"/>
-    </row>
-    <row r="13" spans="1:9" ht="81.75" customHeight="1">
-      <c r="A13" s="152"/>
-      <c r="B13" s="94" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="95" t="s">
-        <v>143</v>
-      </c>
-      <c r="D13" s="96" t="s">
-        <v>89</v>
-      </c>
-      <c r="E13" s="97" t="s">
-        <v>102</v>
-      </c>
-      <c r="F13" s="99" t="s">
-        <v>145</v>
-      </c>
-      <c r="G13" s="121"/>
-      <c r="H13" s="164"/>
+      <c r="G13" s="130"/>
+      <c r="H13" s="104"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -6600,115 +6463,113 @@
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="11.46484375" customWidth="1"/>
-    <col min="2" max="2" width="19.46484375" customWidth="1"/>
-    <col min="3" max="3" width="19.86328125" customWidth="1"/>
-    <col min="4" max="4" width="21.1328125" customWidth="1"/>
-    <col min="5" max="5" width="26.1328125" customWidth="1"/>
-    <col min="6" max="6" width="50.46484375" customWidth="1"/>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="2" max="2" width="19.5" customWidth="1"/>
+    <col min="3" max="3" width="19.875" customWidth="1"/>
+    <col min="4" max="4" width="21.125" customWidth="1"/>
+    <col min="5" max="5" width="26.125" customWidth="1"/>
+    <col min="6" max="6" width="50.5" customWidth="1"/>
     <col min="7" max="7" width="69" customWidth="1"/>
-    <col min="8" max="8" width="27.1328125" customWidth="1"/>
+    <col min="8" max="8" width="27.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="45.75" customHeight="1" thickBot="1">
-      <c r="A1" s="79"/>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80" t="s">
+    <row r="1" spans="1:8" ht="45.75" customHeight="1" thickBot="1">
+      <c r="A1" s="55"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="80" t="s">
+      <c r="D1" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="80" t="s">
+      <c r="E1" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="80" t="s">
+      <c r="F1" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="80" t="s">
+      <c r="G1" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="81" t="s">
-        <v>111</v>
+      <c r="H1" s="57" t="s">
+        <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="99.75">
-      <c r="A2" s="147" t="s">
-        <v>117</v>
+    <row r="2" spans="1:8" ht="94.5">
+      <c r="A2" s="87" t="s">
+        <v>116</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="G2" s="6"/>
+      <c r="H2" s="74"/>
+    </row>
+    <row r="3" spans="1:8" ht="66" customHeight="1">
+      <c r="A3" s="88"/>
+      <c r="B3" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="122"/>
-      <c r="I2">
-        <v>15</v>
-      </c>
+      <c r="E3" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="G3" s="11"/>
+      <c r="H3" s="75"/>
     </row>
-    <row r="3" spans="1:9" ht="66" customHeight="1">
-      <c r="A3" s="148"/>
-      <c r="B3" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="C3" s="8" t="s">
+    <row r="4" spans="1:8" ht="60" customHeight="1">
+      <c r="A4" s="92"/>
+      <c r="B4" s="115" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="116" t="s">
         <v>120</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D4" s="117" t="s">
         <v>113</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E4" s="118" t="s">
         <v>115</v>
       </c>
-      <c r="F3" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="123"/>
-    </row>
-    <row r="4" spans="1:9" ht="60" customHeight="1">
-      <c r="A4" s="152"/>
-      <c r="B4" s="124" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" s="125" t="s">
-        <v>121</v>
-      </c>
-      <c r="D4" s="126" t="s">
-        <v>114</v>
-      </c>
-      <c r="E4" s="127" t="s">
-        <v>116</v>
-      </c>
-      <c r="F4" s="128" t="s">
-        <v>189</v>
-      </c>
-      <c r="G4" s="129"/>
-      <c r="H4" s="130"/>
+      <c r="F4" s="133" t="s">
+        <v>187</v>
+      </c>
+      <c r="G4" s="134"/>
+      <c r="H4" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Added two members; revised member info; fixed name order and phone number for jp and ch.
</commit_message>
<xml_diff>
--- a/_ux/弁護士紹介 中＋日＋英.xlsx
+++ b/_ux/弁護士紹介 中＋日＋英.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17571"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2655" yWindow="75" windowWidth="20745" windowHeight="11130" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Fukuoka" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="190">
   <si>
     <t>名前</t>
     <rPh sb="0" eb="2">
@@ -141,7 +141,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -341,7 +341,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -352,7 +352,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -362,7 +362,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -439,13 +439,6 @@
   </si>
   <si>
     <t>東京第一弁護士会所属</t>
-  </si>
-  <si>
-    <t>東京第一弁護士会所属</t>
-    <rPh sb="2" eb="4">
-      <t>ダイイチ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t xml:space="preserve">私立武蔵高等学校 卒業
@@ -483,7 +476,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -509,7 +502,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -521,7 +514,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -532,7 +525,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -543,7 +536,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -554,7 +547,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -565,7 +558,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -575,7 +568,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -587,7 +580,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -598,7 +591,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -609,7 +602,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -619,7 +612,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -630,7 +623,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -710,7 +703,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -734,10 +727,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>東京弁護士会所属</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <r>
       <t>东</t>
     </r>
@@ -745,7 +734,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -756,7 +745,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -767,7 +756,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -858,7 +847,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -960,7 +949,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1078,7 +1067,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1089,7 +1078,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1100,7 +1089,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1111,7 +1100,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1122,7 +1111,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1295,7 +1284,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1306,7 +1295,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1440,7 +1429,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1509,7 +1498,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1592,7 +1581,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1603,7 +1592,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1726,7 +1715,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1753,7 +1742,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1785,7 +1774,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1853,7 +1842,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -1865,7 +1854,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1876,7 +1865,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -1887,7 +1876,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1899,7 +1888,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -1910,7 +1899,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1922,7 +1911,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -1933,7 +1922,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1950,7 +1939,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1961,7 +1950,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1971,7 +1960,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1982,7 +1971,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1992,7 +1981,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2003,7 +1992,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2013,7 +2002,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2024,7 +2013,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2034,7 +2023,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2045,7 +2034,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2056,7 +2045,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2067,7 +2056,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2078,7 +2067,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2089,7 +2078,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2099,7 +2088,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2110,7 +2099,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2120,7 +2109,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2133,7 +2122,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2143,7 +2132,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2154,7 +2143,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2164,7 +2153,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2175,7 +2164,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2185,7 +2174,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2196,7 +2185,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2206,7 +2195,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2223,7 +2212,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2234,7 +2223,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2244,7 +2233,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2255,7 +2244,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2266,7 +2255,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2277,7 +2266,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2287,7 +2276,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2298,7 +2287,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2309,7 +2298,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2320,7 +2309,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2357,7 +2346,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2367,7 +2356,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2378,7 +2367,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2396,7 +2385,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2407,7 +2396,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2417,7 +2406,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2428,7 +2417,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2439,7 +2428,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2450,7 +2439,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2460,7 +2449,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2471,7 +2460,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2482,7 +2471,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2493,7 +2482,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2503,7 +2492,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2514,7 +2503,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2536,7 +2525,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2547,7 +2536,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2558,7 +2547,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2569,7 +2558,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2580,7 +2569,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2591,7 +2580,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2602,7 +2591,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2613,7 +2602,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2624,7 +2613,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2635,7 +2624,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2646,7 +2635,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2657,7 +2646,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2668,7 +2657,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2679,7 +2668,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2690,7 +2679,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2701,7 +2690,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2712,7 +2701,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2722,7 +2711,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2733,7 +2722,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2743,7 +2732,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2754,7 +2743,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2764,7 +2753,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2775,7 +2764,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2785,7 +2774,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2796,7 +2785,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2807,7 +2796,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2818,7 +2807,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2829,7 +2818,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2840,7 +2829,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2850,7 +2839,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2861,7 +2850,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2872,7 +2861,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2883,7 +2872,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2894,7 +2883,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2905,7 +2894,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2916,7 +2905,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2927,7 +2916,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2938,7 +2927,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2949,7 +2938,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2960,7 +2949,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2971,7 +2960,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2982,7 +2971,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2992,7 +2981,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3003,7 +2992,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -3013,7 +3002,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3024,7 +3013,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -3098,7 +3087,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3183,7 +3172,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3202,7 +3191,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3213,7 +3202,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3225,7 +3214,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3236,7 +3225,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3247,7 +3236,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3258,7 +3247,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3270,7 +3259,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3281,7 +3270,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3292,7 +3281,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3303,7 +3292,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3315,7 +3304,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3326,7 +3315,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3337,7 +3326,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3348,7 +3337,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3359,7 +3348,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3370,7 +3359,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -3381,7 +3370,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3392,7 +3381,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3403,7 +3392,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3414,7 +3403,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3425,7 +3414,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3436,7 +3425,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3447,7 +3436,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3458,7 +3447,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3469,7 +3458,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3480,7 +3469,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3492,7 +3481,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3503,7 +3492,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3514,7 +3503,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3525,7 +3514,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3536,7 +3525,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3547,7 +3536,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3559,7 +3548,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3570,7 +3559,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3581,7 +3570,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3592,7 +3581,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3603,7 +3592,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3614,7 +3603,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3632,7 +3621,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3643,7 +3632,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -3655,7 +3644,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3666,7 +3655,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -3676,7 +3665,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3687,7 +3676,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -3713,7 +3702,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3729,7 +3718,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -3748,7 +3737,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3759,7 +3748,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3770,7 +3759,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3781,7 +3770,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3793,7 +3782,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3804,7 +3793,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3815,7 +3804,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3826,7 +3815,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3837,7 +3826,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3848,7 +3837,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3859,7 +3848,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3870,7 +3859,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3881,7 +3870,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3892,7 +3881,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3903,7 +3892,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3914,7 +3903,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3926,7 +3915,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3937,7 +3926,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3948,7 +3937,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3959,7 +3948,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3970,7 +3959,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3981,7 +3970,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3993,7 +3982,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -4010,7 +3999,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -4037,7 +4026,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -4058,7 +4047,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -4069,7 +4058,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -4080,23 +4069,26 @@
   <si>
     <t>Commentary on Korean Nationality Law-Yasuhiro Okuda, Katsuhiko Oka, Masataka Kyou -Akashi Publication 2014</t>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>東京弁護士会所属</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -4104,7 +4096,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -4118,7 +4110,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -4126,7 +4118,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -4134,7 +4126,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -4156,7 +4148,7 @@
       <b/>
       <sz val="18"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -4164,7 +4156,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -4173,7 +4165,7 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -4181,14 +4173,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -4196,14 +4188,14 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -5018,6 +5010,96 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5072,99 +5154,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -5180,7 +5172,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office ​​テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -5222,7 +5214,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5255,9 +5247,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5290,6 +5299,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -5468,18 +5494,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView showGridLines="0" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.5" customWidth="1"/>
-    <col min="2" max="2" width="19.5" customWidth="1"/>
-    <col min="3" max="3" width="19.875" customWidth="1"/>
-    <col min="4" max="4" width="21.125" customWidth="1"/>
-    <col min="5" max="5" width="26.125" customWidth="1"/>
-    <col min="6" max="6" width="50.5" customWidth="1"/>
+    <col min="1" max="1" width="11.47265625" customWidth="1"/>
+    <col min="2" max="2" width="19.47265625" customWidth="1"/>
+    <col min="3" max="3" width="19.89453125" customWidth="1"/>
+    <col min="4" max="4" width="21.1015625" customWidth="1"/>
+    <col min="5" max="5" width="26.1015625" customWidth="1"/>
+    <col min="6" max="6" width="50.47265625" customWidth="1"/>
     <col min="7" max="7" width="69" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5503,7 +5529,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="93" customHeight="1">
-      <c r="A2" s="87" t="s">
+      <c r="A2" s="117" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -5519,16 +5545,16 @@
         <v>17</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G2" s="58" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="111" customHeight="1">
-      <c r="A3" s="88"/>
+      <c r="A3" s="118"/>
       <c r="B3" s="7" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>6</v>
@@ -5540,35 +5566,35 @@
         <v>15</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G3" s="59" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="96.75" customHeight="1" thickBot="1">
-      <c r="A4" s="88"/>
-      <c r="B4" s="105" t="s">
+      <c r="A4" s="118"/>
+      <c r="B4" s="87" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="106" t="s">
+      <c r="C4" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="107" t="s">
+      <c r="D4" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="108" t="s">
+      <c r="E4" s="90" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="109" t="s">
-        <v>164</v>
-      </c>
-      <c r="G4" s="110" t="s">
-        <v>156</v>
+      <c r="F4" s="91" t="s">
+        <v>162</v>
+      </c>
+      <c r="G4" s="92" t="s">
+        <v>154</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="67.5">
-      <c r="A5" s="88"/>
+    <row r="5" spans="1:7" ht="72">
+      <c r="A5" s="118"/>
       <c r="B5" s="12" t="s">
         <v>18</v>
       </c>
@@ -5588,8 +5614,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="94.5">
-      <c r="A6" s="88"/>
+    <row r="6" spans="1:7" ht="100.8">
+      <c r="A6" s="118"/>
       <c r="B6" s="16" t="s">
         <v>19</v>
       </c>
@@ -5603,35 +5629,35 @@
         <v>15</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G6" s="61" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="68.25" thickBot="1">
-      <c r="A7" s="88"/>
-      <c r="B7" s="105" t="s">
+    <row r="7" spans="1:7" ht="72.3" thickBot="1">
+      <c r="A7" s="118"/>
+      <c r="B7" s="87" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="106" t="s">
-        <v>91</v>
-      </c>
-      <c r="D7" s="107" t="s">
+      <c r="C7" s="88" t="s">
+        <v>89</v>
+      </c>
+      <c r="D7" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="108" t="s">
+      <c r="E7" s="90" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="111" t="s">
+      <c r="F7" s="93" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="112" t="s">
-        <v>157</v>
+      <c r="G7" s="94" t="s">
+        <v>155</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="67.5">
-      <c r="A8" s="88"/>
+    <row r="8" spans="1:7" ht="86.4">
+      <c r="A8" s="118"/>
       <c r="B8" s="21" t="s">
         <v>30</v>
       </c>
@@ -5643,14 +5669,14 @@
         <v>32</v>
       </c>
       <c r="F8" s="66" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G8" s="62" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="63.75" customHeight="1">
-      <c r="A9" s="88"/>
+      <c r="A9" s="118"/>
       <c r="B9" s="26" t="s">
         <v>19</v>
       </c>
@@ -5664,33 +5690,33 @@
         <v>36</v>
       </c>
       <c r="F9" s="29" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G9" s="63" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="66.75" customHeight="1" thickBot="1">
-      <c r="A10" s="88"/>
-      <c r="B10" s="105" t="s">
+      <c r="A10" s="118"/>
+      <c r="B10" s="87" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="106" t="s">
+      <c r="C10" s="88" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="107"/>
-      <c r="E10" s="108" t="s">
-        <v>163</v>
-      </c>
-      <c r="F10" s="111" t="s">
-        <v>178</v>
-      </c>
-      <c r="G10" s="113" t="s">
-        <v>175</v>
+      <c r="D10" s="89"/>
+      <c r="E10" s="90" t="s">
+        <v>161</v>
+      </c>
+      <c r="F10" s="93" t="s">
+        <v>176</v>
+      </c>
+      <c r="G10" s="95" t="s">
+        <v>173</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="81">
-      <c r="A11" s="88"/>
+    <row r="11" spans="1:7" ht="86.4">
+      <c r="A11" s="118"/>
       <c r="B11" s="37" t="s">
         <v>18</v>
       </c>
@@ -5704,19 +5730,19 @@
         <v>39</v>
       </c>
       <c r="F11" s="33" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G11" s="64" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="67.5" customHeight="1">
-      <c r="A12" s="88"/>
+      <c r="A12" s="118"/>
       <c r="B12" s="39" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="34" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D12" s="35" t="s">
         <v>24</v>
@@ -5725,90 +5751,90 @@
         <v>40</v>
       </c>
       <c r="F12" s="36" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G12" s="65" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="74.25" customHeight="1" thickBot="1">
-      <c r="A13" s="88"/>
-      <c r="B13" s="105" t="s">
+      <c r="A13" s="118"/>
+      <c r="B13" s="87" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="106" t="s">
+      <c r="C13" s="88" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="107" t="s">
+      <c r="D13" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="108" t="s">
+      <c r="E13" s="90" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="111" t="s">
-        <v>124</v>
-      </c>
-      <c r="G13" s="114" t="s">
+      <c r="F13" s="93" t="s">
+        <v>122</v>
+      </c>
+      <c r="G13" s="96" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="302.39999999999998">
+      <c r="A14" s="119" t="s">
+        <v>132</v>
+      </c>
+      <c r="B14" s="77" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="243">
-      <c r="A14" s="89" t="s">
+      <c r="C14" s="78" t="s">
         <v>134</v>
-      </c>
-      <c r="B14" s="77" t="s">
-        <v>135</v>
-      </c>
-      <c r="C14" s="78" t="s">
-        <v>136</v>
       </c>
       <c r="D14" s="79"/>
       <c r="E14" s="78" t="s">
         <v>17</v>
       </c>
       <c r="F14" s="80" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G14" s="81" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="267.75" customHeight="1">
-      <c r="A15" s="90"/>
+      <c r="A15" s="120"/>
       <c r="B15" s="82" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C15" s="83" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D15" s="84"/>
       <c r="E15" s="83" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F15" s="85" t="s">
+        <v>166</v>
+      </c>
+      <c r="G15" s="86" t="s">
         <v>168</v>
-      </c>
-      <c r="G15" s="86" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="204.75" customHeight="1">
-      <c r="A16" s="91"/>
-      <c r="B16" s="115" t="s">
+      <c r="A16" s="121"/>
+      <c r="B16" s="97" t="s">
+        <v>136</v>
+      </c>
+      <c r="C16" s="98" t="s">
         <v>138</v>
       </c>
-      <c r="C16" s="116" t="s">
-        <v>140</v>
-      </c>
-      <c r="D16" s="117"/>
-      <c r="E16" s="118" t="s">
-        <v>102</v>
-      </c>
-      <c r="F16" s="119" t="s">
-        <v>179</v>
-      </c>
-      <c r="G16" s="120" t="s">
-        <v>174</v>
+      <c r="D16" s="99"/>
+      <c r="E16" s="100" t="s">
+        <v>100</v>
+      </c>
+      <c r="F16" s="101" t="s">
+        <v>177</v>
+      </c>
+      <c r="G16" s="102" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -5826,18 +5852,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:G16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.5" customWidth="1"/>
-    <col min="2" max="2" width="19.5" customWidth="1"/>
-    <col min="3" max="3" width="19.875" customWidth="1"/>
-    <col min="4" max="4" width="23.875" customWidth="1"/>
-    <col min="5" max="5" width="26.125" customWidth="1"/>
-    <col min="6" max="6" width="52.875" customWidth="1"/>
+    <col min="1" max="1" width="11.47265625" customWidth="1"/>
+    <col min="2" max="2" width="19.47265625" customWidth="1"/>
+    <col min="3" max="3" width="19.89453125" customWidth="1"/>
+    <col min="4" max="4" width="23.89453125" customWidth="1"/>
+    <col min="5" max="5" width="26.1015625" customWidth="1"/>
+    <col min="6" max="6" width="52.89453125" customWidth="1"/>
     <col min="7" max="7" width="69" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5861,7 +5887,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="120" customHeight="1" thickBot="1">
-      <c r="A2" s="87" t="s">
+      <c r="A2" s="117" t="s">
         <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -5871,67 +5897,67 @@
         <v>45</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>17</v>
       </c>
       <c r="F2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="136.5" customHeight="1" thickBot="1">
-      <c r="A3" s="88"/>
+      <c r="A3" s="118"/>
       <c r="B3" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>15</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G3" s="52" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="114" customHeight="1" thickBot="1">
-      <c r="A4" s="88"/>
-      <c r="B4" s="105" t="s">
+      <c r="A4" s="118"/>
+      <c r="B4" s="87" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="88" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="106" t="s">
+      <c r="D4" s="89" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="107" t="s">
+      <c r="E4" s="90" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="91" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="108" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="109" t="s">
-        <v>55</v>
-      </c>
-      <c r="G4" s="121" t="s">
-        <v>166</v>
+      <c r="G4" s="103" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="77.25" customHeight="1">
-      <c r="A5" s="88"/>
+      <c r="A5" s="118"/>
       <c r="B5" s="12" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>46</v>
@@ -5940,74 +5966,74 @@
         <v>17</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G5" s="60"/>
     </row>
     <row r="6" spans="1:7" ht="95.25" customHeight="1">
-      <c r="A6" s="88"/>
+      <c r="A6" s="118"/>
       <c r="B6" s="16" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E6" s="17" t="s">
         <v>15</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G6" s="61"/>
     </row>
     <row r="7" spans="1:7" ht="84" customHeight="1" thickBot="1">
-      <c r="A7" s="88"/>
-      <c r="B7" s="105" t="s">
+      <c r="A7" s="118"/>
+      <c r="B7" s="87" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="106" t="s">
+      <c r="C7" s="88" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="89" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="90" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="93" t="s">
         <v>60</v>
       </c>
-      <c r="D7" s="107" t="s">
-        <v>54</v>
-      </c>
-      <c r="E7" s="108" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="111" t="s">
-        <v>61</v>
-      </c>
-      <c r="G7" s="112"/>
+      <c r="G7" s="94"/>
     </row>
     <row r="8" spans="1:7" ht="62.25" customHeight="1">
-      <c r="A8" s="88"/>
+      <c r="A8" s="118"/>
       <c r="B8" s="21" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>64</v>
+        <v>189</v>
       </c>
       <c r="E8" s="22" t="s">
         <v>17</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G8" s="67"/>
     </row>
     <row r="9" spans="1:7" ht="75.75" customHeight="1">
-      <c r="A9" s="88"/>
+      <c r="A9" s="118"/>
       <c r="B9" s="26" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D9" s="28" t="s">
         <v>13</v>
@@ -6016,36 +6042,36 @@
         <v>15</v>
       </c>
       <c r="F9" s="29" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G9" s="63"/>
     </row>
     <row r="10" spans="1:7" ht="81.75" customHeight="1" thickBot="1">
-      <c r="A10" s="88"/>
-      <c r="B10" s="105" t="s">
+      <c r="A10" s="118"/>
+      <c r="B10" s="87" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="106" t="s">
-        <v>66</v>
-      </c>
-      <c r="D10" s="107" t="s">
-        <v>65</v>
-      </c>
-      <c r="E10" s="108" t="s">
+      <c r="C10" s="88" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="89" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="90" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="122" t="s">
-        <v>151</v>
-      </c>
-      <c r="G10" s="112"/>
+      <c r="F10" s="104" t="s">
+        <v>149</v>
+      </c>
+      <c r="G10" s="94"/>
     </row>
     <row r="11" spans="1:7" ht="89.25" customHeight="1">
-      <c r="A11" s="88"/>
+      <c r="A11" s="118"/>
       <c r="B11" s="37" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D11" s="32" t="s">
         <v>11</v>
@@ -6054,97 +6080,97 @@
         <v>17</v>
       </c>
       <c r="F11" s="33" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G11" s="68"/>
     </row>
     <row r="12" spans="1:7" ht="104.25" customHeight="1">
-      <c r="A12" s="88"/>
+      <c r="A12" s="118"/>
       <c r="B12" s="39" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="34" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D12" s="35" t="s">
         <v>13</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F12" s="36" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G12" s="65"/>
     </row>
     <row r="13" spans="1:7" ht="81.75" customHeight="1" thickBot="1">
-      <c r="A13" s="88"/>
-      <c r="B13" s="123" t="s">
+      <c r="A13" s="118"/>
+      <c r="B13" s="105" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="124" t="s">
-        <v>71</v>
-      </c>
-      <c r="D13" s="125" t="s">
-        <v>68</v>
-      </c>
-      <c r="E13" s="126" t="s">
+      <c r="C13" s="106" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="107" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="108" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="127" t="s">
-        <v>152</v>
-      </c>
-      <c r="G13" s="128"/>
+      <c r="F13" s="109" t="s">
+        <v>150</v>
+      </c>
+      <c r="G13" s="110"/>
     </row>
     <row r="14" spans="1:7" ht="87.75" customHeight="1">
       <c r="A14" s="72"/>
       <c r="B14" s="41" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C14" s="42" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D14" s="43"/>
       <c r="E14" s="42" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F14" s="44" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G14" s="45"/>
     </row>
     <row r="15" spans="1:7" ht="89.25" customHeight="1">
       <c r="B15" s="46" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C15" s="47" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D15" s="48"/>
       <c r="E15" s="47" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F15" s="49" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G15" s="50"/>
     </row>
     <row r="16" spans="1:7" ht="108" customHeight="1">
       <c r="A16" s="73"/>
-      <c r="B16" s="115" t="s">
-        <v>77</v>
-      </c>
-      <c r="C16" s="116" t="s">
-        <v>78</v>
-      </c>
-      <c r="D16" s="117"/>
-      <c r="E16" s="118" t="s">
-        <v>82</v>
-      </c>
-      <c r="F16" s="129" t="s">
-        <v>155</v>
-      </c>
-      <c r="G16" s="130"/>
+      <c r="B16" s="97" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="98" t="s">
+        <v>76</v>
+      </c>
+      <c r="D16" s="99"/>
+      <c r="E16" s="100" t="s">
+        <v>80</v>
+      </c>
+      <c r="F16" s="111" t="s">
+        <v>153</v>
+      </c>
+      <c r="G16" s="112"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6159,20 +6185,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.5" customWidth="1"/>
-    <col min="2" max="2" width="19.5" customWidth="1"/>
-    <col min="3" max="3" width="19.875" customWidth="1"/>
-    <col min="4" max="4" width="21.125" customWidth="1"/>
-    <col min="5" max="5" width="16.625" customWidth="1"/>
-    <col min="6" max="6" width="54.625" customWidth="1"/>
-    <col min="7" max="7" width="64.375" customWidth="1"/>
-    <col min="8" max="8" width="47.25" customWidth="1"/>
+    <col min="1" max="1" width="11.47265625" customWidth="1"/>
+    <col min="2" max="2" width="19.47265625" customWidth="1"/>
+    <col min="3" max="3" width="19.89453125" customWidth="1"/>
+    <col min="4" max="4" width="21.1015625" customWidth="1"/>
+    <col min="5" max="5" width="16.62890625" customWidth="1"/>
+    <col min="6" max="6" width="54.62890625" customWidth="1"/>
+    <col min="7" max="7" width="64.3671875" customWidth="1"/>
+    <col min="8" max="8" width="47.26171875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="43.5" customHeight="1" thickBot="1">
@@ -6194,264 +6220,264 @@
         <v>4</v>
       </c>
       <c r="H1" s="57" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="135" customHeight="1">
-      <c r="A2" s="87" t="s">
-        <v>83</v>
+      <c r="A2" s="117" t="s">
+        <v>81</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>86</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>17</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G2" s="53" t="s">
-        <v>185</v>
-      </c>
-      <c r="H2" s="93" t="s">
-        <v>106</v>
+        <v>183</v>
+      </c>
+      <c r="H2" s="123" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="108.75" customHeight="1">
-      <c r="A3" s="88"/>
+      <c r="A3" s="118"/>
       <c r="B3" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>15</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G3" s="54" t="s">
-        <v>172</v>
-      </c>
-      <c r="H3" s="94"/>
+        <v>170</v>
+      </c>
+      <c r="H3" s="124"/>
     </row>
     <row r="4" spans="1:8" ht="147" customHeight="1" thickBot="1">
-      <c r="A4" s="88"/>
-      <c r="B4" s="105" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" s="106" t="s">
-        <v>88</v>
-      </c>
-      <c r="D4" s="107" t="s">
-        <v>94</v>
-      </c>
-      <c r="E4" s="108" t="s">
+      <c r="A4" s="118"/>
+      <c r="B4" s="87" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="88" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="89" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" s="90" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="109" t="s">
-        <v>183</v>
-      </c>
-      <c r="G4" s="131" t="s">
-        <v>184</v>
-      </c>
-      <c r="H4" s="95"/>
+      <c r="F4" s="91" t="s">
+        <v>181</v>
+      </c>
+      <c r="G4" s="113" t="s">
+        <v>182</v>
+      </c>
+      <c r="H4" s="125"/>
     </row>
     <row r="5" spans="1:8" ht="77.25" customHeight="1">
-      <c r="A5" s="88"/>
+      <c r="A5" s="118"/>
       <c r="B5" s="12" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G5" s="51"/>
-      <c r="H5" s="96" t="s">
-        <v>107</v>
+      <c r="H5" s="126" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="248.25" customHeight="1">
-      <c r="A6" s="88"/>
+      <c r="A6" s="118"/>
       <c r="B6" s="16" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E6" s="17" t="s">
         <v>15</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G6" s="20"/>
-      <c r="H6" s="97"/>
+      <c r="H6" s="127"/>
     </row>
     <row r="7" spans="1:8" ht="140.25" customHeight="1" thickBot="1">
-      <c r="A7" s="88"/>
-      <c r="B7" s="105" t="s">
+      <c r="A7" s="118"/>
+      <c r="B7" s="87" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="106" t="s">
-        <v>97</v>
-      </c>
-      <c r="D7" s="107" t="s">
-        <v>89</v>
-      </c>
-      <c r="E7" s="108" t="s">
+      <c r="C7" s="88" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" s="89" t="s">
+        <v>87</v>
+      </c>
+      <c r="E7" s="90" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="111" t="s">
+      <c r="F7" s="93" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="131"/>
-      <c r="H7" s="98"/>
+      <c r="G7" s="113"/>
+      <c r="H7" s="128"/>
     </row>
     <row r="8" spans="1:8" ht="140.25" customHeight="1">
-      <c r="A8" s="88"/>
+      <c r="A8" s="118"/>
       <c r="B8" s="21" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" s="23" t="s">
         <v>99</v>
-      </c>
-      <c r="D8" s="23" t="s">
-        <v>101</v>
       </c>
       <c r="E8" s="22" t="s">
         <v>17</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G8" s="25"/>
-      <c r="H8" s="99" t="s">
-        <v>108</v>
+      <c r="H8" s="129" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="103.5" customHeight="1">
-      <c r="A9" s="88"/>
+      <c r="A9" s="118"/>
       <c r="B9" s="26" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E9" s="27" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F9" s="29" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G9" s="30"/>
-      <c r="H9" s="100"/>
+      <c r="H9" s="130"/>
     </row>
     <row r="10" spans="1:8" ht="81.75" customHeight="1" thickBot="1">
-      <c r="A10" s="88"/>
-      <c r="B10" s="105" t="s">
-        <v>150</v>
-      </c>
-      <c r="C10" s="106" t="s">
-        <v>149</v>
-      </c>
-      <c r="D10" s="107" t="s">
-        <v>89</v>
-      </c>
-      <c r="E10" s="108" t="s">
+      <c r="A10" s="118"/>
+      <c r="B10" s="87" t="s">
+        <v>148</v>
+      </c>
+      <c r="C10" s="88" t="s">
+        <v>147</v>
+      </c>
+      <c r="D10" s="89" t="s">
+        <v>87</v>
+      </c>
+      <c r="E10" s="90" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="111" t="s">
-        <v>147</v>
-      </c>
-      <c r="G10" s="132"/>
-      <c r="H10" s="101"/>
+      <c r="F10" s="93" t="s">
+        <v>145</v>
+      </c>
+      <c r="G10" s="114"/>
+      <c r="H10" s="131"/>
     </row>
     <row r="11" spans="1:8" ht="84.75" customHeight="1">
-      <c r="A11" s="88"/>
+      <c r="A11" s="118"/>
       <c r="B11" s="37" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D11" s="32" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E11" s="31" t="s">
         <v>17</v>
       </c>
       <c r="F11" s="33" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G11" s="38"/>
-      <c r="H11" s="102" t="s">
-        <v>109</v>
+      <c r="H11" s="132" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="94.5" customHeight="1">
-      <c r="A12" s="88"/>
+      <c r="A12" s="118"/>
       <c r="B12" s="39" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="D12" s="35" t="s">
+        <v>158</v>
+      </c>
+      <c r="E12" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" s="36" t="s">
         <v>141</v>
       </c>
-      <c r="D12" s="35" t="s">
-        <v>160</v>
-      </c>
-      <c r="E12" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="F12" s="36" t="s">
-        <v>143</v>
-      </c>
       <c r="G12" s="40"/>
-      <c r="H12" s="103"/>
+      <c r="H12" s="133"/>
     </row>
     <row r="13" spans="1:8" ht="81.75" customHeight="1">
-      <c r="A13" s="92"/>
-      <c r="B13" s="115" t="s">
+      <c r="A13" s="122"/>
+      <c r="B13" s="97" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="116" t="s">
+      <c r="C13" s="98" t="s">
+        <v>140</v>
+      </c>
+      <c r="D13" s="99" t="s">
+        <v>87</v>
+      </c>
+      <c r="E13" s="100" t="s">
+        <v>100</v>
+      </c>
+      <c r="F13" s="101" t="s">
         <v>142</v>
       </c>
-      <c r="D13" s="117" t="s">
-        <v>89</v>
-      </c>
-      <c r="E13" s="118" t="s">
-        <v>102</v>
-      </c>
-      <c r="F13" s="119" t="s">
-        <v>144</v>
-      </c>
-      <c r="G13" s="130"/>
-      <c r="H13" s="104"/>
+      <c r="G13" s="112"/>
+      <c r="H13" s="134"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -6471,20 +6497,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.5" customWidth="1"/>
-    <col min="2" max="2" width="19.5" customWidth="1"/>
-    <col min="3" max="3" width="19.875" customWidth="1"/>
-    <col min="4" max="4" width="21.125" customWidth="1"/>
-    <col min="5" max="5" width="26.125" customWidth="1"/>
-    <col min="6" max="6" width="50.5" customWidth="1"/>
+    <col min="1" max="1" width="11.47265625" customWidth="1"/>
+    <col min="2" max="2" width="19.47265625" customWidth="1"/>
+    <col min="3" max="3" width="19.89453125" customWidth="1"/>
+    <col min="4" max="4" width="21.1015625" customWidth="1"/>
+    <col min="5" max="5" width="26.1015625" customWidth="1"/>
+    <col min="6" max="6" width="50.47265625" customWidth="1"/>
     <col min="7" max="7" width="69" customWidth="1"/>
-    <col min="8" max="8" width="27.125" customWidth="1"/>
+    <col min="8" max="8" width="27.1015625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="45.75" customHeight="1" thickBot="1">
@@ -6506,69 +6532,69 @@
         <v>4</v>
       </c>
       <c r="H1" s="57" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="94.5">
-      <c r="A2" s="87" t="s">
-        <v>116</v>
+    <row r="2" spans="1:8" ht="100.8">
+      <c r="A2" s="117" t="s">
+        <v>114</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G2" s="6"/>
       <c r="H2" s="74"/>
     </row>
     <row r="3" spans="1:8" ht="66" customHeight="1">
-      <c r="A3" s="88"/>
+      <c r="A3" s="118"/>
       <c r="B3" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D3" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>114</v>
-      </c>
       <c r="F3" s="10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="75"/>
     </row>
     <row r="4" spans="1:8" ht="60" customHeight="1">
-      <c r="A4" s="92"/>
-      <c r="B4" s="115" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" s="116" t="s">
-        <v>120</v>
-      </c>
-      <c r="D4" s="117" t="s">
+      <c r="A4" s="122"/>
+      <c r="B4" s="97" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="98" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="99" t="s">
+        <v>111</v>
+      </c>
+      <c r="E4" s="100" t="s">
         <v>113</v>
       </c>
-      <c r="E4" s="118" t="s">
-        <v>115</v>
-      </c>
-      <c r="F4" s="133" t="s">
-        <v>187</v>
-      </c>
-      <c r="G4" s="134"/>
+      <c r="F4" s="115" t="s">
+        <v>185</v>
+      </c>
+      <c r="G4" s="116"/>
       <c r="H4" s="76"/>
     </row>
   </sheetData>

</xml_diff>